<commit_message>
DB design & Menu style fix
</commit_message>
<xml_diff>
--- a/designDB.xlsx
+++ b/designDB.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
   <si>
     <t xml:space="preserve">users</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t xml:space="preserve">password_hash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
   </si>
   <si>
     <t xml:space="preserve">bio</t>
@@ -211,11 +214,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -248,16 +255,20 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -354,13 +365,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:G22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K26" activeCellId="0" sqref="K26"/>
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.14"/>
@@ -368,173 +379,344 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.78"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="E2" s="1" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="D3" s="1"/>
+      <c r="E3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2"/>
-      <c r="B4" s="7" t="s">
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3"/>
+      <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="C4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-      <c r="B5" s="7" t="s">
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3"/>
+      <c r="B5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="C5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
-      <c r="B6" s="7" t="s">
+      <c r="F5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3"/>
+      <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="C6" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2"/>
-      <c r="B7" s="7" t="s">
+      <c r="F6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
+      <c r="B7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
-      <c r="B8" s="7" t="s">
+      <c r="C7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="7" t="s">
+      <c r="F7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3"/>
+      <c r="B8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="7" t="s">
+      <c r="C8" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1"/>
+      <c r="B9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="7" t="s">
+      <c r="C9" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+      <c r="B10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>5</v>
-      </c>
+      <c r="C10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+      <c r="B11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="E18" s="9" t="s">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="A19" s="1"/>
+      <c r="B19" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="10" t="s">
+      <c r="D19" s="1"/>
+      <c r="E19" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G19" s="10"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="12" t="s">
+      <c r="A20" s="1"/>
+      <c r="B20" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="13" t="s">
+      <c r="D20" s="1"/>
+      <c r="E20" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G20" s="13"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E21" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F21" s="10" t="s">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="F21" s="13" t="s">
         <v>23</v>
       </c>
+      <c r="G21" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E22" s="14"/>
-      <c r="F22" s="15"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>